<commit_message>
fixed index renaming for neural net
</commit_message>
<xml_diff>
--- a/mean_results/avg_tpe_train_results_80_20.xlsx
+++ b/mean_results/avg_tpe_train_results_80_20.xlsx
@@ -1216,12 +1216,12 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A27:A31"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
     <mergeCell ref="A32:A36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
box plot with Bayesian Results
</commit_message>
<xml_diff>
--- a/mean_results/avg_tpe_train_results_80_20.xlsx
+++ b/mean_results/avg_tpe_train_results_80_20.xlsx
@@ -1320,14 +1320,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A27:A31"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
     <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A32:A36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
final cleanup, README, Demo.ipynb, results
</commit_message>
<xml_diff>
--- a/mean_results/avg_tpe_train_results_80_20.xlsx
+++ b/mean_results/avg_tpe_train_results_80_20.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,45 +489,45 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>DecisionTreeClassifier</t>
+          <t>LGBMClassifier</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6066666666666667</v>
+        <v>0.8685362969196534</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5</v>
+        <v>0.8530612244897959</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5377272727272727</v>
+        <v>0.8596347786884143</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6634920634920635</v>
+        <v>0.846838213546288</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7285714285714285</v>
+        <v>0.859090909090909</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6905219780219781</v>
+        <v>0.8516318002896168</v>
       </c>
       <c r="F3" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.8559139784946236</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.8559139784946236</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.8559139784946236</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.8559139784946236</v>
       </c>
     </row>
     <row r="5">
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.635079365079365</v>
+        <v>0.8576872552329707</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6142857142857142</v>
+        <v>0.8560760667903524</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6141246253746253</v>
+        <v>0.8556332894890156</v>
       </c>
       <c r="F5" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
@@ -578,60 +578,60 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6398148148148148</v>
+        <v>0.8582705370440827</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.8559139784946236</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6268575174825175</v>
+        <v>0.8558484233169402</v>
       </c>
       <c r="F6" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>NeuralNetClassifier</t>
+          <t>RandomForestClassifier</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4697435897435898</v>
+        <v>0.847704991087344</v>
       </c>
       <c r="D7" t="n">
-        <v>0.54</v>
+        <v>0.8775510204081632</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4999385155906895</v>
+        <v>0.8619016653449643</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6612554112554113</v>
+        <v>0.858312447786132</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6</v>
+        <v>0.8227272727272726</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6264908424908425</v>
+        <v>0.8394360990905441</v>
       </c>
       <c r="F8" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -642,16 +642,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.575</v>
+        <v>0.8516129032258064</v>
       </c>
       <c r="D9" t="n">
-        <v>0.575</v>
+        <v>0.8516129032258064</v>
       </c>
       <c r="E9" t="n">
-        <v>0.575</v>
+        <v>0.8516129032258064</v>
       </c>
       <c r="F9" t="n">
-        <v>0.575</v>
+        <v>0.8516129032258064</v>
       </c>
     </row>
     <row r="10">
@@ -662,16 +662,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5654995004995005</v>
+        <v>0.8530087194367379</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5700000000000001</v>
+        <v>0.8501391465677181</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5632146790407659</v>
+        <v>0.8506688822177543</v>
       </c>
       <c r="F10" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
@@ -682,60 +682,60 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.581458818958819</v>
+        <v>0.8527235727512867</v>
       </c>
       <c r="D11" t="n">
-        <v>0.575</v>
+        <v>0.8516129032258064</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5737607062824455</v>
+        <v>0.8512727952891096</v>
       </c>
       <c r="F11" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>ElasticNet</t>
+          <t>NeuralNetClassifier</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.4811965811965813</v>
+        <v>0.6874934498871716</v>
       </c>
       <c r="D12" t="n">
-        <v>0.52</v>
+        <v>0.8653061224489796</v>
       </c>
       <c r="E12" t="n">
-        <v>0.496692323694612</v>
+        <v>0.7613981552700898</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6272727272727272</v>
+        <v>0.796369239622613</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5857142857142857</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6032466843501326</v>
+        <v>0.6331356371938563</v>
       </c>
       <c r="F13" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
@@ -746,16 +746,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.7139784946236559</v>
       </c>
     </row>
     <row r="15">
@@ -766,16 +766,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.5542346542346543</v>
+        <v>0.7419313447548923</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5528571428571428</v>
+        <v>0.7053803339517625</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5499695040223723</v>
+        <v>0.697266896231973</v>
       </c>
       <c r="F15" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16">
@@ -786,60 +786,60 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.5664076664076665</v>
+        <v>0.739004576213617</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.7139784946236559</v>
       </c>
       <c r="E16" t="n">
-        <v>0.558849034076999</v>
+        <v>0.70071481338456</v>
       </c>
       <c r="F16" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>LGBMClassifier</t>
+          <t>DecisionTreeClassifier</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.4501373626373626</v>
+        <v>0.6882132813905231</v>
       </c>
       <c r="D17" t="n">
-        <v>0.54</v>
+        <v>0.7755102040816326</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4834188829073739</v>
+        <v>0.7226024384647601</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6184046345811052</v>
+        <v>0.7197823860727086</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5285714285714286</v>
+        <v>0.5954545454545455</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5620951951274532</v>
+        <v>0.6372805332194786</v>
       </c>
       <c r="F18" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19">
@@ -850,16 +850,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6903225806451613</v>
       </c>
     </row>
     <row r="20">
@@ -870,16 +870,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.534270998609234</v>
+        <v>0.7039978337316158</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5342857142857144</v>
+        <v>0.685482374768089</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5227570390174135</v>
+        <v>0.6799414858421194</v>
       </c>
       <c r="F20" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -890,60 +890,60 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.5482932712712125</v>
+        <v>0.7031492018853206</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5293133983690869</v>
+        <v>0.6822350854454873</v>
       </c>
       <c r="F21" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>RandomForestClassifier</t>
+          <t>LinearBoostClassifier</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.4141258741258741</v>
+        <v>0.6904106280193237</v>
       </c>
       <c r="D22" t="n">
-        <v>0.46</v>
+        <v>0.6571428571428571</v>
       </c>
       <c r="E22" t="n">
-        <v>0.434824016563147</v>
+        <v>0.6732510592119694</v>
       </c>
       <c r="F22" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5877122877122878</v>
+        <v>0.6387647754137116</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5428571428571429</v>
+        <v>0.6727272727272727</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5633227513227513</v>
+        <v>0.6551925358471523</v>
       </c>
       <c r="F23" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24">
@@ -954,16 +954,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.5083333333333333</v>
+        <v>0.664516129032258</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5083333333333333</v>
+        <v>0.664516129032258</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5083333333333333</v>
+        <v>0.664516129032258</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5083333333333333</v>
+        <v>0.664516129032258</v>
       </c>
     </row>
     <row r="25">
@@ -974,16 +974,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.5009190809190809</v>
+        <v>0.6645877017165176</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5014285714285714</v>
+        <v>0.6649350649350649</v>
       </c>
       <c r="E25" t="n">
-        <v>0.4990733839429492</v>
+        <v>0.6642217975295608</v>
       </c>
       <c r="F25" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26">
@@ -994,60 +994,60 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5153846153846154</v>
+        <v>0.6659760310876363</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5083333333333333</v>
+        <v>0.664516129032258</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5097816118395829</v>
+        <v>0.6647072417060345</v>
       </c>
       <c r="F26" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>SVC</t>
+          <t>XGBClassifier</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.4141176470588235</v>
+        <v>0.8</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5599999999999999</v>
+        <v>0.4122448979591836</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4723367003367003</v>
+        <v>0.5395279673801024</v>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.6095238095238095</v>
+        <v>0.6171252133400451</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4571428571428571</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5149705367096671</v>
+        <v>0.7597273097622192</v>
       </c>
       <c r="F28" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29">
@@ -1058,16 +1058,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.5</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5</v>
+        <v>0.6903225806451613</v>
       </c>
     </row>
     <row r="30">
@@ -1078,16 +1078,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.5118207282913165</v>
+        <v>0.7085626066700226</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5085714285714286</v>
+        <v>0.7061224489795919</v>
       </c>
       <c r="E30" t="n">
-        <v>0.4936536185231837</v>
+        <v>0.6496276385711608</v>
       </c>
       <c r="F30" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31">
@@ -1098,60 +1098,60 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.5281045751633988</v>
+        <v>0.7134785955587311</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5</v>
+        <v>0.6903225806451613</v>
       </c>
       <c r="E31" t="n">
-        <v>0.4972064382209309</v>
+        <v>0.6437083014103513</v>
       </c>
       <c r="F31" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>LogisticRegression</t>
+          <t>ElasticNet</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.3381196581196581</v>
+        <v>0.6430986863002752</v>
       </c>
       <c r="D32" t="n">
-        <v>0.38</v>
+        <v>0.7061224489795919</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3555148741418764</v>
+        <v>0.6728246923299885</v>
       </c>
       <c r="F32" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.5873160173160172</v>
+        <v>0.6336562784420801</v>
       </c>
       <c r="D33" t="n">
-        <v>0.6285714285714286</v>
+        <v>0.5636363636363637</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5937920663728287</v>
+        <v>0.5960855750286982</v>
       </c>
       <c r="F33" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34">
@@ -1162,16 +1162,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.525</v>
+        <v>0.6387096774193548</v>
       </c>
       <c r="D34" t="n">
-        <v>0.525</v>
+        <v>0.6387096774193548</v>
       </c>
       <c r="E34" t="n">
-        <v>0.525</v>
+        <v>0.6387096774193548</v>
       </c>
       <c r="F34" t="n">
-        <v>0.525</v>
+        <v>0.6387096774193548</v>
       </c>
     </row>
     <row r="35">
@@ -1182,16 +1182,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.4627178377178377</v>
+        <v>0.6383774823711776</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5042857142857142</v>
+        <v>0.6348794063079778</v>
       </c>
       <c r="E35" t="n">
-        <v>0.4746534702573525</v>
+        <v>0.6344551336793434</v>
       </c>
       <c r="F35" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36">
@@ -1202,60 +1202,60 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.483484200984201</v>
+        <v>0.6386313105394088</v>
       </c>
       <c r="D36" t="n">
-        <v>0.525</v>
+        <v>0.6387096774193548</v>
       </c>
       <c r="E36" t="n">
-        <v>0.4945099029432652</v>
+        <v>0.6365180131766899</v>
       </c>
       <c r="F36" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>XGBClassifier</t>
+          <t>SVC</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>Did not Play: 0</t>
+          <t>No Prior Concussion: 0</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.3511111111111111</v>
+        <v>0.5934526856559148</v>
       </c>
       <c r="D37" t="n">
-        <v>0.14</v>
+        <v>0.6612244897959184</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1682934609250399</v>
+        <v>0.6232929866098293</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>Played in the NHL: 1</t>
+          <t>Prior Concussion: 1</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.5817641930914241</v>
+        <v>0.59195388164417</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8428571428571429</v>
+        <v>0.509090909090909</v>
       </c>
       <c r="E38" t="n">
-        <v>0.6835772138131484</v>
+        <v>0.5434946657915315</v>
       </c>
       <c r="F38" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39">
@@ -1266,16 +1266,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.55</v>
+        <v>0.589247311827957</v>
       </c>
       <c r="D39" t="n">
-        <v>0.55</v>
+        <v>0.589247311827957</v>
       </c>
       <c r="E39" t="n">
-        <v>0.55</v>
+        <v>0.589247311827957</v>
       </c>
       <c r="F39" t="n">
-        <v>0.55</v>
+        <v>0.589247311827957</v>
       </c>
     </row>
     <row r="40">
@@ -1286,16 +1286,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.4664376521012678</v>
+        <v>0.5927032836500424</v>
       </c>
       <c r="D40" t="n">
-        <v>0.4914285714285714</v>
+        <v>0.5851576994434138</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4259353373690941</v>
+        <v>0.5833938262006805</v>
       </c>
       <c r="F40" t="n">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41">
@@ -1306,25 +1306,130 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.4856587422662938</v>
+        <v>0.5927435740804656</v>
       </c>
       <c r="D41" t="n">
-        <v>0.55</v>
+        <v>0.589247311827957</v>
       </c>
       <c r="E41" t="n">
-        <v>0.4688756501097699</v>
+        <v>0.5855389423517099</v>
       </c>
       <c r="F41" t="n">
-        <v>24</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>LogisticRegression</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>No Prior Concussion: 0</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.4915584415584416</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.499760612005901</v>
+      </c>
+      <c r="F42" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n"/>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>Prior Concussion: 1</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.5560418685517033</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.6409090909090909</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.5782509282044364</v>
+      </c>
+      <c r="F43" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n"/>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.5720430107526882</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.5720430107526882</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.5720430107526882</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.5720430107526882</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n"/>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>macro avg</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.5238001550550725</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.5755565862708719</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.5390057701051687</v>
+      </c>
+      <c r="F45" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n"/>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>weighted avg</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.5220667295982644</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.5720430107526882</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.5368958153686488</v>
+      </c>
+      <c r="F46" t="n">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A42:A46"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A32:A36"/>

</xml_diff>